<commit_message>
took buttons off of pages. modifications to excel template
</commit_message>
<xml_diff>
--- a/assets/template_pl.xlsx
+++ b/assets/template_pl.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James McCartney\PycharmProjects\BCI_Database_Builder\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A7CD256-BDB5-40EB-8A93-9ADCDBC3F7CB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83520FCC-35CA-4537-8C81-ED9CA4D59078}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="IO" sheetId="3" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Type</t>
   </si>
@@ -53,10 +53,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Reference</t>
+    <t>DA/RA</t>
   </si>
   <si>
-    <t>DA/RA</t>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Instance</t>
+  </si>
+  <si>
+    <t>Configuration</t>
   </si>
 </sst>
 </file>
@@ -475,16 +481,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34D82697-CD2F-48E5-A04A-2055E57EB6B4}">
   <dimension ref="A1:E1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -499,10 +505,10 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
   </sheetData>
@@ -512,41 +518,89 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FAA74904-653A-4461-88FE-1C220F15F51A}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.42578125" bestFit="1" customWidth="1"/>
   </cols>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{724E0D88-7BF2-4134-BFF8-CB2F588C66DD}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24215C1B-6E35-4D39-90BB-C7E57BA57F58}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <dimension ref="A1:C1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>